<commit_message>
Updated with new versions of login, and search
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84CEC87-6AE6-4750-A52C-0DCCB27D7F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959CFDD3-5D1B-4EF9-873C-E93F8A9E2873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
+    <sheet name="Shay" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>Cage Id</t>
   </si>
@@ -465,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1435,4 +1436,398 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4">
+        <v>98216</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="9">
+        <v>44045</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4">
+        <v>97213</v>
+      </c>
+      <c r="N2" s="4">
+        <v>97345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="4">
+        <v>97123</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="9">
+        <v>43711</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="4">
+        <v>93456</v>
+      </c>
+      <c r="N3" s="4">
+        <v>93453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4">
+        <v>97235</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="9">
+        <v>43137</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="4">
+        <v>92345</v>
+      </c>
+      <c r="N4" s="4">
+        <v>92456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed cage, new welcome user and more
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959CFDD3-5D1B-4EF9-873C-E93F8A9E2873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3497127A-8910-4723-B23A-EAF6D3AC6B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
     <sheet name="Shay" sheetId="2" r:id="rId2"/>
+    <sheet name="Shay12" sheetId="3" r:id="rId3"/>
+    <sheet name="Shay11" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1442,7 +1444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1830,4 +1832,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491D9DA1-1B41-4BAE-A235-2A59F31BEF0A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3804BE-B17F-43D1-B03C-3B03FAACAF66}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding a way to destinguish between adults and offsprings
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AECAB7A-EB1D-49D1-9527-1831CC293375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8A154C-5B59-4039-A578-73AA64500128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2925" yWindow="2400" windowWidth="17010" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Cage Id</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>24/08/2022</t>
+  </si>
+  <si>
+    <t>offspring</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -498,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
@@ -1472,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,7 +1494,7 @@
     <col min="11" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1526,8 +1535,11 @@
       <c r="N1" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O1" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1568,8 +1580,11 @@
       <c r="N2" s="4">
         <v>97345</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1600,8 +1615,11 @@
       <c r="N3" s="4">
         <v>93453</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1632,8 +1650,11 @@
       <c r="N4" s="4">
         <v>92456</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1649,7 +1670,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1665,7 +1686,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1679,7 +1700,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1693,7 +1714,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1707,7 +1728,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1721,7 +1742,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1735,7 +1756,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1749,7 +1770,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1763,7 +1784,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1777,7 +1798,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1791,7 +1812,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>

</xml_diff>

<commit_message>
when adding a bird or a cage the counter in the top nav bar will increment
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8A154C-5B59-4039-A578-73AA64500128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7E9633-DA00-4150-A388-6D78B94FAD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2925" yWindow="2400" windowWidth="17010" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Cage Id</t>
   </si>
@@ -126,6 +126,27 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>asd123</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>qwe123</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1483,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,11 +1606,21 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="4">
         <v>97123</v>
@@ -1620,11 +1651,21 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="G4" s="4">
         <v>97235</v>

</xml_diff>

<commit_message>
adding a better version of a date for addBird window
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC20DC80-CA77-4240-BE82-DD21B6E28BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37CF8AF-9BDE-4D6B-8668-4F56790F4E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2925" yWindow="2400" windowWidth="17010" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1484,7 +1484,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="A3:E4"/>
+      <selection activeCell="O5" sqref="G5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new method that checks offspring values
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37CF8AF-9BDE-4D6B-8668-4F56790F4E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816BF718-3812-41A6-85A0-3D6765D71C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="2400" windowWidth="17010" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -1483,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O5" sqref="G5:O5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed some minor bugs, still need to fix the date in the moreDetails window
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816BF718-3812-41A6-85A0-3D6765D71C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C0A084-F45C-4ADF-91F1-3EB32373EA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="2400" windowWidth="17010" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Cage Id</t>
   </si>
@@ -116,9 +116,6 @@
     <t>08/01/2022</t>
   </si>
   <si>
-    <t>24/08/2022</t>
-  </si>
-  <si>
     <t>offspring</t>
   </si>
   <si>
@@ -126,6 +123,24 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Center Australia</t>
+  </si>
+  <si>
+    <t>03/08/2022</t>
+  </si>
+  <si>
+    <t>97235</t>
+  </si>
+  <si>
+    <t>92345</t>
+  </si>
+  <si>
+    <t>92456</t>
+  </si>
+  <si>
+    <t>01/03/2023</t>
   </si>
 </sst>
 </file>
@@ -1483,13 +1498,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="20.7109375" customWidth="1"/>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="12" customWidth="1"/>
     <col min="11" max="12" width="20.7109375" customWidth="1"/>
   </cols>
@@ -1536,7 +1553,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1581,7 +1598,7 @@
         <v>97345</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1616,7 +1633,7 @@
         <v>93453</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1626,17 +1643,17 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="4">
-        <v>97235</v>
+      <c r="G4" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>15</v>
@@ -1644,14 +1661,14 @@
       <c r="L4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="4">
-        <v>92345</v>
-      </c>
-      <c r="N4" s="4">
-        <v>92456</v>
+      <c r="M4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1661,14 +1678,33 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="G5" s="4">
+        <v>97236</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="4">
+        <v>66542</v>
+      </c>
+      <c r="N5" s="4">
+        <v>68859</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>

</xml_diff>

<commit_message>
fixed the issue with sort, now works fine
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05B8871-E7AD-44B0-AA49-79927FA0CD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D5813E-116B-4E22-B6C2-D1A18D57832F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Cage Id</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>Offspring</t>
+  </si>
+  <si>
+    <t>45327</t>
+  </si>
+  <si>
+    <t>14/04/2023</t>
+  </si>
+  <si>
+    <t>98722</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1589,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
       <c r="G2" s="4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>18</v>
@@ -1589,7 +1598,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>14</v>
@@ -1598,13 +1607,13 @@
         <v>12</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1615,28 +1624,28 @@
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>31</v>
@@ -1649,17 +1658,17 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="4">
-        <v>98722</v>
+      <c r="G4" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>15</v>
@@ -1668,10 +1677,10 @@
         <v>12</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>31</v>
@@ -1679,6 +1688,33 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F5" s="11"/>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>

</xml_diff>

<commit_message>
fixed search, opens now more detailes if 1 option
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76228C51-76CA-4F89-8E95-6D49895D27DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE1058D-9C9E-4751-A0A2-EB2125DBC7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
   <si>
     <t>Cage Id</t>
   </si>
@@ -206,15 +206,6 @@
     <t>12/10/2020</t>
   </si>
   <si>
-    <t>1222</t>
-  </si>
-  <si>
-    <t>1002</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
     <t>99972</t>
   </si>
   <si>
@@ -227,25 +218,16 @@
     <t>92223</t>
   </si>
   <si>
-    <t>1005</t>
-  </si>
-  <si>
     <t>87432</t>
   </si>
   <si>
     <t>87631</t>
   </si>
   <si>
-    <t>1010</t>
-  </si>
-  <si>
     <t>90213</t>
   </si>
   <si>
     <t>97322</t>
-  </si>
-  <si>
-    <t>1100</t>
   </si>
   <si>
     <t>10102</t>
@@ -1631,7 +1613,7 @@
   <dimension ref="A1:O93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,8 +1642,8 @@
         <v>13</v>
       </c>
       <c r="F1" s="5"/>
-      <c r="G1" s="13" t="s">
-        <v>61</v>
+      <c r="G1" s="13">
+        <v>10001</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>18</v>
@@ -1679,10 +1661,10 @@
         <v>48</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O1" s="13" t="s">
         <v>31</v>
@@ -1705,8 +1687,8 @@
         <v>52</v>
       </c>
       <c r="F2" s="5"/>
-      <c r="G2" s="13" t="s">
-        <v>60</v>
+      <c r="G2" s="13">
+        <v>10002</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>18</v>
@@ -1724,10 +1706,10 @@
         <v>48</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>31</v>
@@ -1750,8 +1732,8 @@
         <v>53</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="13" t="s">
-        <v>66</v>
+      <c r="G3" s="13">
+        <v>10005</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>18</v>
@@ -1769,10 +1751,10 @@
         <v>49</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>31</v>
@@ -1795,8 +1777,8 @@
         <v>13</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="13" t="s">
-        <v>69</v>
+      <c r="G4" s="13">
+        <v>10010</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>16</v>
@@ -1814,10 +1796,10 @@
         <v>49</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="O4" s="13" t="s">
         <v>31</v>
@@ -1840,8 +1822,8 @@
         <v>52</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="15" t="s">
-        <v>72</v>
+      <c r="G5" s="15">
+        <v>11000</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>20</v>
@@ -1859,10 +1841,10 @@
         <v>48</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="O5" s="15" t="s">
         <v>31</v>
@@ -1875,8 +1857,8 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="13" t="s">
-        <v>59</v>
+      <c r="G6" s="13">
+        <v>12202</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>18</v>
@@ -1893,11 +1875,11 @@
       <c r="L6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>61</v>
+      <c r="M6" s="13">
+        <v>10002</v>
+      </c>
+      <c r="N6" s="13">
+        <v>10001</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
fixing a small typo
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D5813E-116B-4E22-B6C2-D1A18D57832F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C52E7C-1DC4-4BF0-83E2-A602EE93AC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9540" yWindow="4935" windowWidth="13110" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>Cage Id</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>98722</t>
+  </si>
+  <si>
+    <t>Center Australia</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -1525,13 +1528,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="20.7109375" customWidth="1"/>
+    <col min="1" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="10" customWidth="1"/>
     <col min="11" max="12" width="20.7109375" customWidth="1"/>
   </cols>
@@ -1665,7 +1670,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
A  lot of changes to implementation of  program
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC387895-4089-499A-A6E9-F4A3F18CCE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E050A3F-D8E8-4E74-A14C-276CF1FFCCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="86">
   <si>
     <t>Cage Id</t>
   </si>
@@ -134,12 +134,6 @@
     <t>97123</t>
   </si>
   <si>
-    <t>97213</t>
-  </si>
-  <si>
-    <t>97345</t>
-  </si>
-  <si>
     <t>93456</t>
   </si>
   <si>
@@ -164,125 +158,140 @@
     <t>Offspring</t>
   </si>
   <si>
+    <t>14/04/2023</t>
+  </si>
+  <si>
+    <t>98722</t>
+  </si>
+  <si>
+    <t>D534AG</t>
+  </si>
+  <si>
+    <t>C9342G</t>
+  </si>
+  <si>
+    <t>A33S8G</t>
+  </si>
+  <si>
+    <t>D367YU</t>
+  </si>
+  <si>
+    <t>PLASTIC</t>
+  </si>
+  <si>
+    <t>METAL</t>
+  </si>
+  <si>
+    <t>02/05/2023</t>
+  </si>
+  <si>
+    <t>14/08/2023</t>
+  </si>
+  <si>
+    <t>09/01/2022</t>
+  </si>
+  <si>
+    <t>20/08/2022</t>
+  </si>
+  <si>
+    <t>12/10/2020</t>
+  </si>
+  <si>
+    <t>99972</t>
+  </si>
+  <si>
+    <t>28883</t>
+  </si>
+  <si>
+    <t>93356</t>
+  </si>
+  <si>
+    <t>92223</t>
+  </si>
+  <si>
+    <t>87432</t>
+  </si>
+  <si>
+    <t>87631</t>
+  </si>
+  <si>
+    <t>90213</t>
+  </si>
+  <si>
+    <t>97322</t>
+  </si>
+  <si>
+    <t>10102</t>
+  </si>
+  <si>
+    <t>10256</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>10002</t>
+  </si>
+  <si>
+    <t>10005</t>
+  </si>
+  <si>
+    <t>10010</t>
+  </si>
+  <si>
+    <t>11000</t>
+  </si>
+  <si>
+    <t>12202</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>12202,</t>
+  </si>
+  <si>
+    <t>12345,</t>
+  </si>
+  <si>
+    <t>45327,</t>
+  </si>
+  <si>
+    <t>45327,12345,</t>
+  </si>
+  <si>
     <t>45327</t>
   </si>
   <si>
-    <t>14/04/2023</t>
-  </si>
-  <si>
-    <t>98722</t>
-  </si>
-  <si>
-    <t>D534AG</t>
-  </si>
-  <si>
-    <t>C9342G</t>
-  </si>
-  <si>
-    <t>A33S8G</t>
-  </si>
-  <si>
-    <t>D367YU</t>
-  </si>
-  <si>
-    <t>PLASTIC</t>
-  </si>
-  <si>
-    <t>METAL</t>
-  </si>
-  <si>
-    <t>02/05/2023</t>
-  </si>
-  <si>
-    <t>14/08/2023</t>
-  </si>
-  <si>
-    <t>09/01/2022</t>
-  </si>
-  <si>
-    <t>20/08/2022</t>
-  </si>
-  <si>
-    <t>12/10/2020</t>
-  </si>
-  <si>
-    <t>99972</t>
-  </si>
-  <si>
-    <t>28883</t>
-  </si>
-  <si>
-    <t>93356</t>
-  </si>
-  <si>
-    <t>92223</t>
-  </si>
-  <si>
-    <t>87432</t>
-  </si>
-  <si>
-    <t>87631</t>
-  </si>
-  <si>
-    <t>90213</t>
-  </si>
-  <si>
-    <t>97322</t>
-  </si>
-  <si>
-    <t>10102</t>
-  </si>
-  <si>
-    <t>10256</t>
-  </si>
-  <si>
-    <t>10001</t>
-  </si>
-  <si>
-    <t>10002</t>
-  </si>
-  <si>
-    <t>10005</t>
-  </si>
-  <si>
-    <t>10010</t>
-  </si>
-  <si>
-    <t>11000</t>
-  </si>
-  <si>
-    <t>12202</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>360</t>
+    <t>none</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +328,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -349,10 +365,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,9 +411,18 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -732,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1652,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,17 +1691,18 @@
     <col min="11" max="12" width="20.7109375" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.7109375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
@@ -1685,7 +1712,7 @@
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>18</v>
@@ -1694,25 +1721,28 @@
         <v>19</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O1" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="P1" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1720,17 +1750,17 @@
         <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>18</v>
@@ -1739,43 +1769,46 @@
         <v>19</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="P2" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>18</v>
@@ -1784,43 +1817,46 @@
         <v>19</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="P3" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>16</v>
@@ -1829,30 +1865,33 @@
         <v>17</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O4" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P4" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>24</v>
@@ -1861,11 +1900,11 @@
         <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>20</v>
@@ -1874,25 +1913,28 @@
         <v>21</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O5" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="P5" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1900,7 +1942,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
       <c r="G6" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>18</v>
@@ -1909,25 +1951,28 @@
         <v>19</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="P6" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1953,16 +1998,19 @@
         <v>12</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O7" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="P7" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1970,7 +2018,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="13" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>18</v>
@@ -1979,7 +2027,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>14</v>
@@ -1991,13 +2039,16 @@
         <v>34</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O8" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="P8" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2023,16 +2074,19 @@
         <v>12</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O9" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P9" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2040,7 +2094,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>20</v>
@@ -2058,16 +2112,19 @@
         <v>12</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O10" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P10" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2075,7 +2132,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
       <c r="G11" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>18</v>
@@ -2093,16 +2150,19 @@
         <v>12</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O11" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P11" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2118,8 +2178,9 @@
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
-    </row>
-    <row r="13" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P12" s="22"/>
+    </row>
+    <row r="13" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2135,8 +2196,9 @@
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
-    </row>
-    <row r="14" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P13" s="22"/>
+    </row>
+    <row r="14" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2152,8 +2214,9 @@
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P14" s="22"/>
+    </row>
+    <row r="15" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2169,8 +2232,9 @@
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
-    </row>
-    <row r="16" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P15" s="22"/>
+    </row>
+    <row r="16" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2186,8 +2250,9 @@
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
-    </row>
-    <row r="17" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P16" s="22"/>
+    </row>
+    <row r="17" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2203,8 +2268,9 @@
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
-    </row>
-    <row r="18" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P17" s="22"/>
+    </row>
+    <row r="18" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2220,8 +2286,9 @@
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
-    </row>
-    <row r="19" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P18" s="22"/>
+    </row>
+    <row r="19" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2237,8 +2304,9 @@
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
-    </row>
-    <row r="20" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P19" s="22"/>
+    </row>
+    <row r="20" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2254,8 +2322,9 @@
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
-    </row>
-    <row r="21" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F21" s="10"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
@@ -2266,8 +2335,9 @@
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
-    </row>
-    <row r="22" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P21" s="22"/>
+    </row>
+    <row r="22" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F22" s="10"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -2278,8 +2348,9 @@
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-    </row>
-    <row r="23" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P22" s="22"/>
+    </row>
+    <row r="23" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F23" s="10"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -2290,8 +2361,9 @@
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
-    </row>
-    <row r="24" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P23" s="22"/>
+    </row>
+    <row r="24" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F24" s="10"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -2302,8 +2374,9 @@
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
-    </row>
-    <row r="25" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P24" s="22"/>
+    </row>
+    <row r="25" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F25" s="10"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -2314,8 +2387,9 @@
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
-    </row>
-    <row r="26" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P25" s="22"/>
+    </row>
+    <row r="26" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F26" s="10"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -2326,8 +2400,9 @@
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
-    </row>
-    <row r="27" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P26" s="22"/>
+    </row>
+    <row r="27" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F27" s="10"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -2338,8 +2413,9 @@
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
-    </row>
-    <row r="28" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P27" s="22"/>
+    </row>
+    <row r="28" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F28" s="10"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -2350,8 +2426,9 @@
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
-    </row>
-    <row r="29" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P28" s="22"/>
+    </row>
+    <row r="29" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F29" s="10"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -2362,8 +2439,9 @@
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
-    </row>
-    <row r="30" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P29" s="22"/>
+    </row>
+    <row r="30" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F30" s="10"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -2374,8 +2452,9 @@
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
-    </row>
-    <row r="31" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P30" s="22"/>
+    </row>
+    <row r="31" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F31" s="10"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -2386,8 +2465,9 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
-    </row>
-    <row r="32" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P31" s="22"/>
+    </row>
+    <row r="32" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F32" s="10"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -2398,8 +2478,9 @@
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
-    </row>
-    <row r="33" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P32" s="22"/>
+    </row>
+    <row r="33" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F33" s="10"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
@@ -2410,8 +2491,9 @@
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
-    </row>
-    <row r="34" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P33" s="22"/>
+    </row>
+    <row r="34" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F34" s="10"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -2422,8 +2504,9 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
-    </row>
-    <row r="35" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P34" s="22"/>
+    </row>
+    <row r="35" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F35" s="10"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
@@ -2434,8 +2517,9 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
-    </row>
-    <row r="36" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P35" s="22"/>
+    </row>
+    <row r="36" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F36" s="10"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
@@ -2446,8 +2530,9 @@
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
-    </row>
-    <row r="37" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P36" s="22"/>
+    </row>
+    <row r="37" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F37" s="10"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
@@ -2458,8 +2543,9 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
-    </row>
-    <row r="38" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P37" s="22"/>
+    </row>
+    <row r="38" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F38" s="10"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
@@ -2470,8 +2556,9 @@
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
-    </row>
-    <row r="39" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P38" s="22"/>
+    </row>
+    <row r="39" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F39" s="10"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
@@ -2482,8 +2569,9 @@
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
-    </row>
-    <row r="40" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P39" s="22"/>
+    </row>
+    <row r="40" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F40" s="10"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
@@ -2494,8 +2582,9 @@
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P40" s="22"/>
+    </row>
+    <row r="41" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F41" s="10"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
@@ -2506,8 +2595,9 @@
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
       <c r="O41" s="15"/>
-    </row>
-    <row r="42" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P41" s="22"/>
+    </row>
+    <row r="42" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F42" s="10"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
@@ -2518,8 +2608,9 @@
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
       <c r="O42" s="15"/>
-    </row>
-    <row r="43" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P42" s="22"/>
+    </row>
+    <row r="43" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F43" s="10"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
@@ -2530,8 +2621,9 @@
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
       <c r="O43" s="15"/>
-    </row>
-    <row r="44" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P43" s="22"/>
+    </row>
+    <row r="44" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F44" s="10"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
@@ -2542,8 +2634,9 @@
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
       <c r="O44" s="15"/>
-    </row>
-    <row r="45" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P44" s="22"/>
+    </row>
+    <row r="45" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F45" s="10"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
@@ -2554,8 +2647,9 @@
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
-    </row>
-    <row r="46" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P45" s="22"/>
+    </row>
+    <row r="46" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F46" s="10"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
@@ -2566,8 +2660,9 @@
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
-    </row>
-    <row r="47" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P46" s="22"/>
+    </row>
+    <row r="47" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F47" s="10"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
@@ -2578,8 +2673,9 @@
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
       <c r="O47" s="15"/>
-    </row>
-    <row r="48" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P47" s="22"/>
+    </row>
+    <row r="48" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F48" s="10"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
@@ -2590,8 +2686,9 @@
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
       <c r="O48" s="15"/>
-    </row>
-    <row r="49" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P48" s="22"/>
+    </row>
+    <row r="49" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F49" s="10"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
@@ -2602,8 +2699,9 @@
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
       <c r="O49" s="15"/>
-    </row>
-    <row r="50" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P49" s="22"/>
+    </row>
+    <row r="50" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F50" s="10"/>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
@@ -2614,8 +2712,9 @@
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
       <c r="O50" s="15"/>
-    </row>
-    <row r="51" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P50" s="22"/>
+    </row>
+    <row r="51" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F51" s="10"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
@@ -2626,8 +2725,9 @@
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
       <c r="O51" s="15"/>
-    </row>
-    <row r="52" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P51" s="22"/>
+    </row>
+    <row r="52" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F52" s="10"/>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
@@ -2638,8 +2738,9 @@
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
       <c r="O52" s="15"/>
-    </row>
-    <row r="53" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P52" s="22"/>
+    </row>
+    <row r="53" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F53" s="10"/>
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
@@ -2650,8 +2751,9 @@
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
       <c r="O53" s="15"/>
-    </row>
-    <row r="54" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P53" s="22"/>
+    </row>
+    <row r="54" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F54" s="10"/>
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
@@ -2662,8 +2764,9 @@
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
       <c r="O54" s="15"/>
-    </row>
-    <row r="55" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P54" s="22"/>
+    </row>
+    <row r="55" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F55" s="10"/>
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
@@ -2674,8 +2777,9 @@
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
       <c r="O55" s="15"/>
-    </row>
-    <row r="56" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P55" s="22"/>
+    </row>
+    <row r="56" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F56" s="10"/>
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
@@ -2686,8 +2790,9 @@
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
       <c r="O56" s="15"/>
-    </row>
-    <row r="57" spans="6:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="P56" s="22"/>
+    </row>
+    <row r="57" spans="6:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="F57" s="10"/>
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
@@ -2698,8 +2803,9 @@
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
       <c r="O57" s="15"/>
-    </row>
-    <row r="58" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P57" s="22"/>
+    </row>
+    <row r="58" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F58" s="10"/>
       <c r="G58" s="17"/>
       <c r="H58" s="17"/>
@@ -2710,8 +2816,9 @@
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
       <c r="O58" s="17"/>
-    </row>
-    <row r="59" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P58" s="22"/>
+    </row>
+    <row r="59" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F59" s="10"/>
       <c r="G59" s="17"/>
       <c r="H59" s="17"/>
@@ -2722,8 +2829,9 @@
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
       <c r="O59" s="17"/>
-    </row>
-    <row r="60" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P59" s="22"/>
+    </row>
+    <row r="60" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F60" s="10"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -2734,8 +2842,9 @@
       <c r="M60" s="17"/>
       <c r="N60" s="17"/>
       <c r="O60" s="17"/>
-    </row>
-    <row r="61" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P60" s="22"/>
+    </row>
+    <row r="61" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F61" s="10"/>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
@@ -2746,8 +2855,9 @@
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
       <c r="O61" s="17"/>
-    </row>
-    <row r="62" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P61" s="22"/>
+    </row>
+    <row r="62" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F62" s="10"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
@@ -2758,8 +2868,9 @@
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
       <c r="O62" s="17"/>
-    </row>
-    <row r="63" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P62" s="22"/>
+    </row>
+    <row r="63" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F63" s="10"/>
       <c r="G63" s="17"/>
       <c r="H63" s="17"/>
@@ -2770,8 +2881,9 @@
       <c r="M63" s="17"/>
       <c r="N63" s="17"/>
       <c r="O63" s="17"/>
-    </row>
-    <row r="64" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P63" s="22"/>
+    </row>
+    <row r="64" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F64" s="10"/>
       <c r="G64" s="17"/>
       <c r="H64" s="17"/>
@@ -2782,8 +2894,9 @@
       <c r="M64" s="17"/>
       <c r="N64" s="17"/>
       <c r="O64" s="17"/>
-    </row>
-    <row r="65" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P64" s="22"/>
+    </row>
+    <row r="65" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F65" s="10"/>
       <c r="G65" s="17"/>
       <c r="H65" s="17"/>
@@ -2794,8 +2907,9 @@
       <c r="M65" s="17"/>
       <c r="N65" s="17"/>
       <c r="O65" s="17"/>
-    </row>
-    <row r="66" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P65" s="22"/>
+    </row>
+    <row r="66" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F66" s="10"/>
       <c r="G66" s="17"/>
       <c r="H66" s="17"/>
@@ -2806,8 +2920,9 @@
       <c r="M66" s="17"/>
       <c r="N66" s="17"/>
       <c r="O66" s="17"/>
-    </row>
-    <row r="67" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P66" s="22"/>
+    </row>
+    <row r="67" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F67" s="10"/>
       <c r="G67" s="17"/>
       <c r="H67" s="17"/>
@@ -2818,8 +2933,9 @@
       <c r="M67" s="17"/>
       <c r="N67" s="17"/>
       <c r="O67" s="17"/>
-    </row>
-    <row r="68" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P67" s="22"/>
+    </row>
+    <row r="68" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F68" s="10"/>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -2830,8 +2946,9 @@
       <c r="M68" s="17"/>
       <c r="N68" s="17"/>
       <c r="O68" s="17"/>
-    </row>
-    <row r="69" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P68" s="22"/>
+    </row>
+    <row r="69" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F69" s="10"/>
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
@@ -2842,8 +2959,9 @@
       <c r="M69" s="17"/>
       <c r="N69" s="17"/>
       <c r="O69" s="17"/>
-    </row>
-    <row r="70" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P69" s="22"/>
+    </row>
+    <row r="70" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F70" s="10"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
@@ -2854,8 +2972,9 @@
       <c r="M70" s="17"/>
       <c r="N70" s="17"/>
       <c r="O70" s="17"/>
-    </row>
-    <row r="71" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P70" s="22"/>
+    </row>
+    <row r="71" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F71" s="10"/>
       <c r="G71" s="17"/>
       <c r="H71" s="17"/>
@@ -2866,8 +2985,9 @@
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
       <c r="O71" s="17"/>
-    </row>
-    <row r="72" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P71" s="22"/>
+    </row>
+    <row r="72" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F72" s="10"/>
       <c r="G72" s="17"/>
       <c r="H72" s="17"/>
@@ -2878,8 +2998,9 @@
       <c r="M72" s="17"/>
       <c r="N72" s="17"/>
       <c r="O72" s="17"/>
-    </row>
-    <row r="73" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P72" s="22"/>
+    </row>
+    <row r="73" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F73" s="10"/>
       <c r="G73" s="17"/>
       <c r="H73" s="17"/>
@@ -2890,8 +3011,9 @@
       <c r="M73" s="17"/>
       <c r="N73" s="17"/>
       <c r="O73" s="17"/>
-    </row>
-    <row r="74" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P73" s="22"/>
+    </row>
+    <row r="74" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F74" s="10"/>
       <c r="G74" s="17"/>
       <c r="H74" s="17"/>
@@ -2902,8 +3024,9 @@
       <c r="M74" s="17"/>
       <c r="N74" s="17"/>
       <c r="O74" s="17"/>
-    </row>
-    <row r="75" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P74" s="22"/>
+    </row>
+    <row r="75" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F75" s="10"/>
       <c r="G75" s="17"/>
       <c r="H75" s="17"/>
@@ -2914,8 +3037,9 @@
       <c r="M75" s="17"/>
       <c r="N75" s="17"/>
       <c r="O75" s="17"/>
-    </row>
-    <row r="76" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P75" s="22"/>
+    </row>
+    <row r="76" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F76" s="10"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
@@ -2926,8 +3050,9 @@
       <c r="M76" s="17"/>
       <c r="N76" s="17"/>
       <c r="O76" s="17"/>
-    </row>
-    <row r="77" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P76" s="22"/>
+    </row>
+    <row r="77" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F77" s="10"/>
       <c r="G77" s="17"/>
       <c r="H77" s="17"/>
@@ -2938,8 +3063,9 @@
       <c r="M77" s="17"/>
       <c r="N77" s="17"/>
       <c r="O77" s="17"/>
-    </row>
-    <row r="78" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P77" s="22"/>
+    </row>
+    <row r="78" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F78" s="10"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
@@ -2950,8 +3076,9 @@
       <c r="M78" s="17"/>
       <c r="N78" s="17"/>
       <c r="O78" s="17"/>
-    </row>
-    <row r="79" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P78" s="22"/>
+    </row>
+    <row r="79" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F79" s="10"/>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
@@ -2962,8 +3089,9 @@
       <c r="M79" s="17"/>
       <c r="N79" s="17"/>
       <c r="O79" s="17"/>
-    </row>
-    <row r="80" spans="6:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P79" s="22"/>
+    </row>
+    <row r="80" spans="6:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G80" s="17"/>
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
@@ -2973,8 +3101,9 @@
       <c r="M80" s="17"/>
       <c r="N80" s="17"/>
       <c r="O80" s="17"/>
-    </row>
-    <row r="81" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P80" s="22"/>
+    </row>
+    <row r="81" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G81" s="17"/>
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
@@ -2984,8 +3113,9 @@
       <c r="M81" s="17"/>
       <c r="N81" s="17"/>
       <c r="O81" s="17"/>
-    </row>
-    <row r="82" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P81" s="22"/>
+    </row>
+    <row r="82" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G82" s="17"/>
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
@@ -2995,8 +3125,9 @@
       <c r="M82" s="17"/>
       <c r="N82" s="17"/>
       <c r="O82" s="17"/>
-    </row>
-    <row r="83" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P82" s="21"/>
+    </row>
+    <row r="83" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G83" s="17"/>
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
@@ -3006,8 +3137,9 @@
       <c r="M83" s="17"/>
       <c r="N83" s="17"/>
       <c r="O83" s="17"/>
-    </row>
-    <row r="84" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P83" s="21"/>
+    </row>
+    <row r="84" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G84" s="17"/>
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
@@ -3017,8 +3149,9 @@
       <c r="M84" s="17"/>
       <c r="N84" s="17"/>
       <c r="O84" s="17"/>
-    </row>
-    <row r="85" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P84" s="21"/>
+    </row>
+    <row r="85" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G85" s="17"/>
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
@@ -3028,8 +3161,9 @@
       <c r="M85" s="17"/>
       <c r="N85" s="17"/>
       <c r="O85" s="17"/>
-    </row>
-    <row r="86" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P85" s="21"/>
+    </row>
+    <row r="86" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
@@ -3039,8 +3173,9 @@
       <c r="M86" s="11"/>
       <c r="N86" s="11"/>
       <c r="O86" s="11"/>
-    </row>
-    <row r="87" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P86" s="21"/>
+    </row>
+    <row r="87" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
@@ -3050,8 +3185,9 @@
       <c r="M87" s="11"/>
       <c r="N87" s="11"/>
       <c r="O87" s="11"/>
-    </row>
-    <row r="88" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="P87" s="21"/>
+    </row>
+    <row r="88" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="11"/>
@@ -3062,7 +3198,7 @@
       <c r="N88" s="11"/>
       <c r="O88" s="11"/>
     </row>
-    <row r="89" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="89" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="11"/>
@@ -3073,7 +3209,7 @@
       <c r="N89" s="11"/>
       <c r="O89" s="11"/>
     </row>
-    <row r="90" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="90" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="11"/>
@@ -3084,7 +3220,7 @@
       <c r="N90" s="11"/>
       <c r="O90" s="11"/>
     </row>
-    <row r="91" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="91" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="11"/>
@@ -3095,7 +3231,7 @@
       <c r="N91" s="11"/>
       <c r="O91" s="11"/>
     </row>
-    <row r="92" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="92" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
       <c r="I92" s="11"/>
@@ -3106,7 +3242,7 @@
       <c r="N92" s="11"/>
       <c r="O92" s="11"/>
     </row>
-    <row r="93" spans="7:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="93" spans="7:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
       <c r="I93" s="11"/>

</xml_diff>

<commit_message>
updated with new fixes and more functions
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DA18A2-EF78-461A-AAE8-8E084A5FF907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF076B8-2DEC-4D0F-8873-725C70EEC48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
-    <sheet name="Shay" sheetId="2" r:id="rId2"/>
-    <sheet name="Admin" sheetId="3" r:id="rId3"/>
+    <sheet name="Admin" sheetId="3" r:id="rId2"/>
+    <sheet name="Shay" sheetId="2" r:id="rId3"/>
+    <sheet name="Shay12" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="110">
   <si>
     <t>Cage Id</t>
   </si>
@@ -278,13 +279,85 @@
     <t>Center Australia</t>
   </si>
   <si>
-    <t>12345,45327</t>
-  </si>
-  <si>
     <t>02/11/2019</t>
   </si>
   <si>
     <t>09/09/2019</t>
+  </si>
+  <si>
+    <t>AD123</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>11/05/2023</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>98744</t>
+  </si>
+  <si>
+    <t>96666</t>
+  </si>
+  <si>
+    <t>99788</t>
+  </si>
+  <si>
+    <t>99231</t>
+  </si>
+  <si>
+    <t>45678</t>
+  </si>
+  <si>
+    <t>45555</t>
+  </si>
+  <si>
+    <t>90000</t>
+  </si>
+  <si>
+    <t>80006</t>
+  </si>
+  <si>
+    <t>89002</t>
+  </si>
+  <si>
+    <t>90800</t>
+  </si>
+  <si>
+    <t>97777</t>
+  </si>
+  <si>
+    <t>10003</t>
+  </si>
+  <si>
+    <t>10009</t>
+  </si>
+  <si>
+    <t>10007</t>
+  </si>
+  <si>
+    <t>10007|55555|80006|89002|90000|97777</t>
+  </si>
+  <si>
+    <t>10007|55555|80006|89002|90000</t>
+  </si>
+  <si>
+    <t>55555</t>
+  </si>
+  <si>
+    <t>12345|45327</t>
+  </si>
+  <si>
+    <t>Offspring List</t>
   </si>
 </sst>
 </file>
@@ -369,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -419,6 +492,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,7 +777,7 @@
   <dimension ref="A1:X56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -759,6 +833,9 @@
       </c>
       <c r="O1" s="7" t="s">
         <v>42</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>109</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1677,11 +1754,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B058D71E-6C39-4923-84FE-835FB40F9308}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
   <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2190,7 @@
         <v>31</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
@@ -2169,8 +2276,8 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="13">
-        <v>98744</v>
+      <c r="G12" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>16</v>
@@ -2179,7 +2286,7 @@
         <v>17</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>15</v>
@@ -2187,11 +2294,11 @@
       <c r="L12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="15">
-        <v>96666</v>
-      </c>
-      <c r="N12" s="15">
-        <v>99788</v>
+      <c r="M12" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="O12" s="15" t="s">
         <v>31</v>
@@ -2207,8 +2314,8 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="13">
-        <v>99231</v>
+      <c r="G13" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>20</v>
@@ -2217,7 +2324,7 @@
         <v>82</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" s="13" t="s">
         <v>14</v>
@@ -2225,11 +2332,11 @@
       <c r="L13" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="15">
-        <v>45678</v>
-      </c>
-      <c r="N13" s="15">
-        <v>45555</v>
+      <c r="M13" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>96</v>
       </c>
       <c r="O13" s="15" t="s">
         <v>31</v>
@@ -3299,29 +3406,317 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B058D71E-6C39-4923-84FE-835FB40F9308}">
-  <dimension ref="A1:E1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7AAE23-76CB-4482-825A-4943F8FCF709}">
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M6" t="s">
+        <v>102</v>
+      </c>
+      <c r="N6" t="s">
+        <v>103</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" t="s">
+        <v>102</v>
+      </c>
+      <c r="N7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="s">
+        <v>85</v>
+      </c>
+      <c r="M8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N9" t="s">
+        <v>100</v>
+      </c>
+      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no more bugs please
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Database.xlsx
+++ b/ProjectTesting/Excel/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF076B8-2DEC-4D0F-8873-725C70EEC48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F13DAA-8F72-4A5A-978B-00BB30F5D372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="1" r:id="rId1"/>
@@ -777,7 +777,7 @@
   <dimension ref="A1:X56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1787,7 +1787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020368F6-FB6F-4AD2-BF04-86207B5521F0}">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -3410,8 +3410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7AAE23-76CB-4482-825A-4943F8FCF709}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>